<commit_message>
wave speed guesses done
</commit_message>
<xml_diff>
--- a/Notebooks/Exps_summary.xlsx
+++ b/Notebooks/Exps_summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="22">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -40,19 +40,52 @@
     <t xml:space="preserve">Dilution</t>
   </si>
   <si>
+    <t xml:space="preserve">Ti scope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC4100 &amp; DHL708</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pLPT20&amp;pLPT41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10^(-5)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tweez scope</t>
   </si>
   <si>
+    <t xml:space="preserve">10^(-6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DHL708</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pLPT119&amp;pLPT41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC4100 &amp; MG1655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pAAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MG1655</t>
+  </si>
+  <si>
     <t xml:space="preserve">MC4100</t>
   </si>
   <si>
-    <t xml:space="preserve">pLPT20&amp;pLPT41</t>
+    <t xml:space="preserve">pLPT107&amp;pLPT41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPTG</t>
   </si>
   <si>
     <t xml:space="preserve">aTc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10^(-5)</t>
   </si>
 </sst>
 </file>
@@ -241,13 +274,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.71"/>
@@ -279,7 +312,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
-        <v>45268</v>
+        <v>45245</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
@@ -297,18 +330,246 @@
         <v>10</v>
       </c>
     </row>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>45245</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>45247</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>45247</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
+        <v>45260</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
+        <v>45260</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
+        <v>45264</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="n">
+        <v>45264</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="n">
+        <v>45266</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="n">
+        <v>45268</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
+        <v>45268</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
notebooks for thesis updated
</commit_message>
<xml_diff>
--- a/Notebooks/Exps_summary.xlsx
+++ b/Notebooks/Exps_summary.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">IPTG</t>
   </si>
   <si>
-    <t xml:space="preserve">aTc</t>
+    <t xml:space="preserve">ATC</t>
   </si>
 </sst>
 </file>
@@ -277,10 +277,10 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.71"/>

</xml_diff>